<commit_message>
cambios en selection sort y pantalla
</commit_message>
<xml_diff>
--- a/AlgoritmosLCFEstadisticas.xlsx
+++ b/AlgoritmosLCFEstadisticas.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Luis Flores Personal\Luis Flores unitec\2023\Q3\Lenguajes\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\python\ProjectoSorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A83CDF0-7C7E-48AB-8844-F5815D07FB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C00D472-5D0F-46D4-B673-0A83D13DC78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="615" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
   <si>
     <t>SizeArray</t>
   </si>
@@ -46,14 +57,43 @@
   </si>
   <si>
     <t>Bubble Sort</t>
+  </si>
+  <si>
+    <t>Quick sort time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort Algorithm for size Array 10 </t>
+  </si>
+  <si>
+    <t>Tree Sort time</t>
+  </si>
+  <si>
+    <t>Selection Sort time</t>
+  </si>
+  <si>
+    <t>Sort Algorithm for size Array 5</t>
+  </si>
+  <si>
+    <t>Bogo Sort</t>
+  </si>
+  <si>
+    <t>Promedios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,31 +404,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" customWidth="1"/>
-    <col min="12" max="12" width="16.08984375" customWidth="1"/>
-    <col min="13" max="13" width="19.08984375" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" customWidth="1"/>
-    <col min="16" max="16" width="16.90625" customWidth="1"/>
-    <col min="17" max="17" width="12.7265625" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" customWidth="1"/>
-    <col min="19" max="19" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -487,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -537,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -587,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -637,7 +681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -687,7 +731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -737,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -787,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -837,7 +881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -887,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -937,7 +981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I12">
         <v>10</v>
       </c>
@@ -946,6 +990,192 @@
       </c>
       <c r="S12">
         <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D33">
+        <v>2.02</v>
+      </c>
+      <c r="E33">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="G33">
+        <v>14.89</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1.21</v>
+      </c>
+      <c r="D34">
+        <v>2.02</v>
+      </c>
+      <c r="E34">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G34">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1.21</v>
+      </c>
+      <c r="D35">
+        <v>2.02</v>
+      </c>
+      <c r="E35">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G35">
+        <v>28.98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>1.51</v>
+      </c>
+      <c r="D36">
+        <v>2.02</v>
+      </c>
+      <c r="E36">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G36">
+        <v>26.56</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>1.31</v>
+      </c>
+      <c r="D37">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E37">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G37">
+        <v>50.93</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>1.21</v>
+      </c>
+      <c r="D38">
+        <v>2.02</v>
+      </c>
+      <c r="E38">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G38">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>1.41</v>
+      </c>
+      <c r="D39">
+        <v>2.02</v>
+      </c>
+      <c r="E39">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G39">
+        <v>4.83</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>1.41</v>
+      </c>
+      <c r="D40">
+        <v>2.02</v>
+      </c>
+      <c r="E40">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G40">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1.21</v>
+      </c>
+      <c r="D41">
+        <v>2.02</v>
+      </c>
+      <c r="E41">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="G41">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>1.21</v>
+      </c>
+      <c r="D42">
+        <v>2.02</v>
+      </c>
+      <c r="E42">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="G42">
+        <v>28.59</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <f>AVERAGE(C33:C42)</f>
+        <v>1.28</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ref="C44:F44" si="0">AVERAGE(D33:D42)</f>
+        <v>2.0189999999999997</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>9.0380000000000003</v>
+      </c>
+      <c r="G44">
+        <f>AVERAGE(G33:G42)</f>
+        <v>16.828000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>